<commit_message>
Update Program and Check List
</commit_message>
<xml_diff>
--- a/Exams/Exam-01/Program_CheckList.xlsx
+++ b/Exams/Exam-01/Program_CheckList.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="38">
   <si>
     <t>Creterio</t>
   </si>
@@ -111,6 +111,33 @@
   </si>
   <si>
     <t>No hay Proyecto y no se puede ejecutar</t>
+  </si>
+  <si>
+    <t>Se puede simplificar los If</t>
+  </si>
+  <si>
+    <t>Falla en:qwertyuiop, 01012001</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Demasiados If y condiciones largas, en lugar de usar un Switch</t>
+  </si>
+  <si>
+    <t>No hqay retornos directos, hay if and else</t>
+  </si>
+  <si>
+    <t>Oeracionees de Validacion combinadas</t>
+  </si>
+  <si>
+    <t>Hay mucha logica combinada</t>
+  </si>
+  <si>
+    <t>No hay uso de constantse donde si pudiera tnerlas</t>
+  </si>
+  <si>
+    <t>Se complica en algunos momentos por la combinacion de logica en las funciones</t>
   </si>
 </sst>
 </file>
@@ -570,7 +597,7 @@
   <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -603,7 +630,7 @@
         <v>0.5</v>
       </c>
       <c r="C2" s="19">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>28</v>
@@ -617,9 +644,11 @@
         <v>0.5</v>
       </c>
       <c r="C3" s="17">
-        <v>0.5</v>
-      </c>
-      <c r="D3" s="11"/>
+        <v>0.2</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -629,9 +658,11 @@
         <v>1.5</v>
       </c>
       <c r="C4" s="19">
-        <v>1.5</v>
-      </c>
-      <c r="D4" s="2"/>
+        <v>1</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
@@ -641,9 +672,11 @@
         <v>1</v>
       </c>
       <c r="C5" s="17">
-        <v>1</v>
-      </c>
-      <c r="D5" s="11"/>
+        <v>0.8</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
@@ -654,7 +687,7 @@
       </c>
       <c r="C6" s="22">
         <f>SUM(C10:C24)</f>
-        <v>1.5000000000000002</v>
+        <v>0.99999999999999989</v>
       </c>
       <c r="D6" s="2"/>
     </row>
@@ -665,7 +698,7 @@
       <c r="B7" s="15"/>
       <c r="C7" s="16">
         <f>SUM(C2:C6)</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D7" s="15"/>
     </row>
@@ -731,13 +764,15 @@
         <v>13</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="C13" s="5">
         <f t="shared" si="0"/>
-        <v>0.1</v>
-      </c>
-      <c r="D13" s="4"/>
+        <v>0</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
@@ -835,52 +870,60 @@
         <v>22</v>
       </c>
       <c r="B21" s="21" t="s">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="C21" s="5">
         <f t="shared" si="0"/>
-        <v>0.1</v>
-      </c>
-      <c r="D21" s="4"/>
+        <v>0</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
         <v>23</v>
       </c>
       <c r="B22" s="20" t="s">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="C22" s="3">
         <f t="shared" si="0"/>
-        <v>0.1</v>
-      </c>
-      <c r="D22" s="2"/>
+        <v>0</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="18" t="s">
         <v>24</v>
       </c>
       <c r="B23" s="21" t="s">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="C23" s="5">
         <f t="shared" si="0"/>
-        <v>0.1</v>
-      </c>
-      <c r="D23" s="4"/>
+        <v>0</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
         <v>25</v>
       </c>
       <c r="B24" s="20" t="s">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="C24" s="3">
         <f t="shared" si="0"/>
-        <v>0.1</v>
-      </c>
-      <c r="D24" s="2"/>
+        <v>0</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>32</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B10:B24">

</xml_diff>